<commit_message>
deleted the files that we dont use
Left the two blank files as didnt remeber if we are using them or not
</commit_message>
<xml_diff>
--- a/camplist.xlsx
+++ b/camplist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taniaturdean/Desktop/introProgramming/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zuziasosnowska/Documents/GitHub/introProgramming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B5FA96-2F29-F746-AACD-4F8B053A7F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E7CB4D-657E-F942-93C0-2B9D0F5BB5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2320" yWindow="1500" windowWidth="28040" windowHeight="16500" xr2:uid="{CA77FF18-F5A7-5D4B-B023-384DC9E77363}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" xr2:uid="{CA77FF18-F5A7-5D4B-B023-384DC9E77363}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -114,23 +114,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Abadi MT Condensed Light"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Helvetica"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -153,13 +170,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,205 +495,206 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF9AE27-F5FD-6A4C-8805-5F108CB187D1}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="74.33203125" customWidth="1"/>
-    <col min="4" max="4" width="49.83203125" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="74.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.83203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="18" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>43709</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="5">
         <v>43891</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="4">
         <v>100</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="4">
         <v>30</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="4">
         <v>400</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>44713</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>250</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="4">
         <v>50</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="4">
         <v>600</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="6">
         <v>43739</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="6">
         <v>43832</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>50</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>10</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <v>800</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="5" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="6">
         <v>43718</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="6">
         <v>43758</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <v>5</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="3">
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>44718</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <v>20</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <v>3</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="3">
         <v>100</v>
       </c>
     </row>

</xml_diff>